<commit_message>
data modified and done more calculation
</commit_message>
<xml_diff>
--- a/data/raw/长江干流主要观测站点的基本数据.xlsx
+++ b/data/raw/长江干流主要观测站点的基本数据.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Python\05AModel\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Python\05AModel\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E136030-94AA-4970-8EAA-B84E647D6240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6EE843-05AC-4B10-9DF2-93F195E374C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6400" yWindow="1030" windowWidth="19200" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="14">
   <si>
     <t>观测站点</t>
   </si>
@@ -176,6 +176,10 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>2004.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -366,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -401,6 +405,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -413,17 +426,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -708,7 +718,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -719,10 +729,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
@@ -746,10 +756,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="4">
         <v>0</v>
       </c>
@@ -773,7 +783,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="16">
+      <c r="A4" s="13">
         <v>2004.04</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -802,7 +812,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="17"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
@@ -829,7 +839,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="16">
+      <c r="A6" s="13">
         <v>2004.05</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -858,7 +868,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="17"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
@@ -885,7 +895,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16">
+      <c r="A8" s="13">
         <v>2004.06</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -914,7 +924,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="17"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
@@ -941,7 +951,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="16">
+      <c r="A10" s="13">
         <v>2004.07</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -970,7 +980,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="17"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
@@ -997,7 +1007,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="16">
+      <c r="A12" s="13">
         <v>2004.08</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -1026,7 +1036,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="17"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
@@ -1053,7 +1063,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="16">
+      <c r="A14" s="13">
         <v>2004.09</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -1082,7 +1092,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="17"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="6" t="s">
         <v>10</v>
       </c>
@@ -1109,8 +1119,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="16">
-        <v>2004.1</v>
+      <c r="A16" s="20" t="s">
+        <v>13</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>9</v>
@@ -1138,7 +1148,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="17"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="6" t="s">
         <v>10</v>
       </c>
@@ -1165,7 +1175,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="16">
+      <c r="A18" s="13">
         <v>2004.11</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -1194,7 +1204,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="17"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="6" t="s">
         <v>10</v>
       </c>
@@ -1221,7 +1231,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="16">
+      <c r="A20" s="13">
         <v>2004.12</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -1250,7 +1260,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="17"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="6" t="s">
         <v>10</v>
       </c>
@@ -1277,7 +1287,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="16">
+      <c r="A22" s="13">
         <v>2005.01</v>
       </c>
       <c r="B22" s="6" t="s">
@@ -1306,7 +1316,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="17"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="6" t="s">
         <v>10</v>
       </c>
@@ -1333,7 +1343,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="16">
+      <c r="A24" s="13">
         <v>2005.02</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -1362,7 +1372,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="17"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="6" t="s">
         <v>10</v>
       </c>
@@ -1389,7 +1399,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="16">
+      <c r="A26" s="13">
         <v>2005.03</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -1418,7 +1428,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="17"/>
+      <c r="A27" s="14"/>
       <c r="B27" s="6" t="s">
         <v>10</v>
       </c>
@@ -1445,7 +1455,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="16">
+      <c r="A28" s="13">
         <v>2005.04</v>
       </c>
       <c r="B28" s="6" t="s">
@@ -1474,7 +1484,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="18"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="9" t="s">
         <v>10</v>
       </c>
@@ -1501,7 +1511,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="122.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1516,12 +1526,12 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>